<commit_message>
Piccoli aggiustamenti + patch per problema tassative
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_input/Estrazione commesse 5.xlsx
+++ b/PS-VRP/Dati_input/Estrazione commesse 5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wikipedis\Documents\GitHub\progettoIS\PS-VRP\Dati_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frenc\Documents\GitHub\progettoIS\PS-VRP\Dati_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AA8685-D42D-42C8-A164-0F810EDEDF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407A1AC5-3F02-4ABF-8281-2C2B80A56954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -655,7 +655,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -671,7 +671,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>